<commit_message>
Export data to sowing manager
The sowing manager now uses data from the database, as opposed to a default set of values.
</commit_message>
<xml_diff>
--- a/DataFiles/Demo_2_Experiments.xlsx
+++ b/DataFiles/Demo_2_Experiments.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Apsim\REMS\REMS2020\DataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uqmstow1\Documents\GitHub\REMS2020\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17ED77C0-FD09-4458-AB44-CBD068C97BC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37005" yWindow="3135" windowWidth="28215" windowHeight="12420" tabRatio="669" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37005" yWindow="3135" windowWidth="28215" windowHeight="12420" tabRatio="669" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Factors" sheetId="20" r:id="rId1"/>
@@ -218,7 +217,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -445,13 +444,13 @@
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_Design" xfId="4" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Normal_ExperimentInfos" xfId="7" xr:uid="{23F9B8D0-1337-416F-812C-670F03C2CE96}"/>
-    <cellStyle name="Normal_Factors" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal_Irrigation" xfId="5" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Normal_Plots" xfId="6" xr:uid="{E53F5DAC-734B-4365-90A4-6CC1137A9658}"/>
-    <cellStyle name="Normal_Sheet2" xfId="1" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Normal_Sites" xfId="2" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal_Design" xfId="4"/>
+    <cellStyle name="Normal_ExperimentInfos" xfId="7"/>
+    <cellStyle name="Normal_Factors" xfId="3"/>
+    <cellStyle name="Normal_Irrigation" xfId="5"/>
+    <cellStyle name="Normal_Plots" xfId="6"/>
+    <cellStyle name="Normal_Sheet2" xfId="1"/>
+    <cellStyle name="Normal_Sites" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -728,7 +727,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -791,7 +790,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2522,7 +2521,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2605,7 +2604,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2783,7 +2782,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2918,7 +2917,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3011,7 +3010,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3230,7 +3229,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C127"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
@@ -4216,7 +4215,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5259,11 +5258,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B147167-1129-4539-A51B-327E0C86BF99}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5271,8 +5270,8 @@
     <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
     <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4.5703125" bestFit="1" customWidth="1"/>
@@ -5315,7 +5314,7 @@
         <v>57</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E2" s="26" t="s">
         <v>58</v>
@@ -5341,7 +5340,7 @@
         <v>60</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E3" s="26" t="s">
         <v>58</v>
@@ -5362,7 +5361,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
changed cultivar - which doesn't work
</commit_message>
<xml_diff>
--- a/DataFiles/Demo_2_Experiments.xlsx
+++ b/DataFiles/Demo_2_Experiments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Apsim\REMS\REMS2020\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33B31FBB-8B40-4C51-B4D3-13661DAC02F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B5D6C65-1050-4E10-B9E1-09B161B357D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28380" yWindow="4290" windowWidth="28215" windowHeight="12420" tabRatio="669" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37455" yWindow="3435" windowWidth="28215" windowHeight="12420" tabRatio="669" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Factors" sheetId="20" r:id="rId1"/>
@@ -3050,7 +3050,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C25"/>
     </sheetView>
   </sheetViews>
@@ -5372,8 +5372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B147167-1129-4539-A51B-327E0C86BF99}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5425,7 +5425,7 @@
         <v>57</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E2" s="26" t="s">
         <v>58</v>
@@ -5451,7 +5451,7 @@
         <v>60</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E3" s="26" t="s">
         <v>58</v>

</xml_diff>